<commit_message>
Deploying to gh-pages from  @ a26602f6ed394fd9ef862d9f2a2a5aefdeaca22c 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/11.6.1.1a.xlsx
+++ b/en/downloads/data-excel/11.6.1.1a.xlsx
@@ -86,12 +86,20 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -113,6 +121,12 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
@@ -144,38 +158,58 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 5" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -477,9 +511,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
@@ -488,7 +524,7 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -499,7 +535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -510,8 +546,9 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -542,8 +579,11 @@
       <c r="J3" s="5">
         <v>2019</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="9">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -574,8 +614,11 @@
       <c r="J4" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -606,8 +649,11 @@
       <c r="J5" s="1">
         <v>46.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="11">
+        <v>48.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -638,8 +684,11 @@
       <c r="J6" s="1">
         <v>20.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="12">
+        <v>19.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -670,8 +719,11 @@
       <c r="J7" s="8">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K7" s="13">
+        <v>24.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -702,8 +754,11 @@
       <c r="J8" s="7">
         <v>8.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="14">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>

</xml_diff>